<commit_message>
Setup active admin and active storage
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/79efd62cb8f9c5b1/Documents/RRC/FallTerm2020/Adev-2007_FullStack/EcommerceProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C7F1C45A-2B8C-4017-9A8D-FDC0BAD753B3}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="9435" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -814,7 +814,7 @@
       <name val="Consolas"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -831,6 +831,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -861,7 +867,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1007,6 +1013,7 @@
     <xf numFmtId="1" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1485,8 +1492,8 @@
   <dimension ref="A1:AC1121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30:B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1503,7 +1510,7 @@
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; I172 &amp; "  /  Verified: " &amp; J172 &amp; "  /  Verified with Deductions: " &amp; K172 &amp; "  /  Verified with Deductions &amp; Milestones: " &amp; L172</f>
-        <v>Unverified Marks: 4  /  Verified: 4  /  Verified with Deductions: -20  /  Verified with Deductions &amp; Milestones: -20</v>
+        <v>Unverified Marks: 0  /  Verified: 0  /  Verified with Deductions: -30  /  Verified with Deductions &amp; Milestones: -30</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -1618,7 +1625,7 @@
     </row>
     <row r="4" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
-      <c r="B4" s="10"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="23" t="s">
         <v>10</v>
       </c>
@@ -1627,7 +1634,7 @@
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="25" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G4" s="26">
         <v>2</v>
@@ -1637,15 +1644,15 @@
       </c>
       <c r="I4" s="28">
         <f t="shared" ref="I4:I5" si="0">IF(OR(F4 = "maybe", F4 = "yes"),G4, 0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J4" s="28">
         <f t="shared" ref="J4:J5" si="1">IF(F4 = "yes",G4, 0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K4" s="28">
         <f t="shared" ref="K4:K5" si="2">IF(F4 = "yes",G4, $M$2)</f>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
@@ -1668,7 +1675,7 @@
     </row>
     <row r="5" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="23" t="s">
         <v>14</v>
       </c>
@@ -1677,7 +1684,7 @@
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="25" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="G5" s="26">
         <v>2</v>
@@ -1687,15 +1694,15 @@
       </c>
       <c r="I5" s="28">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J5" s="28">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="K5" s="28">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
@@ -1788,7 +1795,7 @@
     </row>
     <row r="8" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
-      <c r="B8" s="10"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="23" t="s">
         <v>18</v>
       </c>
@@ -1836,7 +1843,7 @@
     </row>
     <row r="9" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="23" t="s">
         <v>21</v>
       </c>
@@ -1989,7 +1996,7 @@
     </row>
     <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="23" t="s">
         <v>26</v>
       </c>
@@ -2070,7 +2077,7 @@
     </row>
     <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
-      <c r="B15" s="10"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="23" t="s">
         <v>29</v>
       </c>
@@ -2267,7 +2274,7 @@
     </row>
     <row r="20" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
-      <c r="B20" s="10"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="23" t="s">
         <v>36</v>
       </c>
@@ -2317,7 +2324,7 @@
     </row>
     <row r="21" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
-      <c r="B21" s="10"/>
+      <c r="B21" s="59"/>
       <c r="C21" s="23" t="s">
         <v>38</v>
       </c>
@@ -2435,7 +2442,7 @@
     </row>
     <row r="24" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
-      <c r="B24" s="10"/>
+      <c r="B24" s="59"/>
       <c r="C24" s="23" t="s">
         <v>42</v>
       </c>
@@ -2485,7 +2492,7 @@
     </row>
     <row r="25" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="10"/>
-      <c r="B25" s="10"/>
+      <c r="B25" s="59"/>
       <c r="C25" s="23" t="s">
         <v>44</v>
       </c>
@@ -2673,7 +2680,7 @@
     </row>
     <row r="30" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A30" s="10"/>
-      <c r="B30" s="10"/>
+      <c r="B30" s="59"/>
       <c r="C30" s="36" t="s">
         <v>50</v>
       </c>
@@ -2721,7 +2728,7 @@
     </row>
     <row r="31" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
+      <c r="B31" s="59"/>
       <c r="C31" s="23" t="s">
         <v>52</v>
       </c>
@@ -8105,19 +8112,19 @@
       <c r="H172" s="11"/>
       <c r="I172" s="58">
         <f t="shared" ref="I172:K172" si="23">SUM(I4:I164)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J172" s="28">
         <f t="shared" si="23"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="K172" s="28">
         <f t="shared" si="23"/>
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="L172" s="21">
         <f>CHOOSE(SUM(L167:L170)+1, MIN(60, K172) + (K172 - MIN(60, K172))/2,MIN(70, KJ172) + (K172 - MIN(70, K172))/2,MIN(80, K172) + (K172 - MIN(80, K172))/2,MIN(90, K172) + (K172 - MIN(90, K172))/2, K172)</f>
-        <v>-20</v>
+        <v>-30</v>
       </c>
       <c r="M172" s="22"/>
       <c r="N172" s="8"/>

</xml_diff>

<commit_message>
1.4 added edit of about/contact page
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C7F1C45A-2B8C-4017-9A8D-FDC0BAD753B3}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8D6110DE-3FFF-4960-8F2E-61F438AE1089}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="9435" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="218">
   <si>
     <t>Confirm</t>
   </si>
@@ -702,6 +702,12 @@
   </si>
   <si>
     <t>Yes Sum with Milestones</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -1492,8 +1498,8 @@
   <dimension ref="A1:AC1121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B30" sqref="B30:B31"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1510,7 +1516,7 @@
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; I172 &amp; "  /  Verified: " &amp; J172 &amp; "  /  Verified with Deductions: " &amp; K172 &amp; "  /  Verified with Deductions &amp; Milestones: " &amp; L172</f>
-        <v>Unverified Marks: 0  /  Verified: 0  /  Verified with Deductions: -30  /  Verified with Deductions &amp; Milestones: -30</v>
+        <v>Unverified Marks: 10  /  Verified: 0  /  Verified with Deductions: -30  /  Verified with Deductions &amp; Milestones: -30</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -1634,7 +1640,7 @@
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="25" t="s">
-        <v>20</v>
+        <v>216</v>
       </c>
       <c r="G4" s="26">
         <v>2</v>
@@ -1644,7 +1650,7 @@
       </c>
       <c r="I4" s="28">
         <f t="shared" ref="I4:I5" si="0">IF(OR(F4 = "maybe", F4 = "yes"),G4, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J4" s="28">
         <f t="shared" ref="J4:J5" si="1">IF(F4 = "yes",G4, 0)</f>
@@ -1684,7 +1690,7 @@
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="25" t="s">
-        <v>20</v>
+        <v>216</v>
       </c>
       <c r="G5" s="26">
         <v>2</v>
@@ -1694,7 +1700,7 @@
       </c>
       <c r="I5" s="28">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J5" s="28">
         <f t="shared" si="1"/>
@@ -1804,7 +1810,7 @@
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="25" t="s">
-        <v>20</v>
+        <v>216</v>
       </c>
       <c r="G8" s="26">
         <v>2</v>
@@ -1812,7 +1818,7 @@
       <c r="H8" s="32"/>
       <c r="I8" s="21">
         <f t="shared" ref="I8:I9" si="3">IF(OR(F8 = "maybe", F8 = "yes"),G8, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J8" s="21">
         <f t="shared" ref="J8:J9" si="4">IF(F8 = "yes",G8, 0)</f>
@@ -1852,7 +1858,7 @@
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="25" t="s">
-        <v>20</v>
+        <v>216</v>
       </c>
       <c r="G9" s="26">
         <v>2</v>
@@ -1860,7 +1866,7 @@
       <c r="H9" s="32"/>
       <c r="I9" s="21">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J9" s="21">
         <f t="shared" si="4"/>
@@ -1897,7 +1903,7 @@
         <v>23</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F10" s="30"/>
       <c r="G10" s="31"/>
@@ -1932,7 +1938,7 @@
         <v>24</v>
       </c>
       <c r="E11" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F11" s="30"/>
       <c r="G11" s="31"/>
@@ -1967,7 +1973,7 @@
         <v>25</v>
       </c>
       <c r="E12" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F12" s="30"/>
       <c r="G12" s="31"/>
@@ -2005,7 +2011,7 @@
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="25" t="s">
-        <v>20</v>
+        <v>216</v>
       </c>
       <c r="G13" s="26">
         <v>2</v>
@@ -2013,7 +2019,7 @@
       <c r="H13" s="32"/>
       <c r="I13" s="21">
         <f>IF(OR(F13 = "maybe", F13 = "yes"),G13, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J13" s="21">
         <f>IF(F13 = "yes",G13, 0)</f>
@@ -7807,13 +7813,15 @@
       </c>
       <c r="E164" s="47"/>
       <c r="F164" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="G164" s="46"/>
+        <v>216</v>
+      </c>
+      <c r="G164" s="46" t="s">
+        <v>217</v>
+      </c>
       <c r="H164" s="32"/>
-      <c r="I164" s="21">
+      <c r="I164" s="21" t="str">
         <f>IF(OR(F164 = "maybe", F164 = "yes"),G164, 0)</f>
-        <v>0</v>
+        <v>??</v>
       </c>
       <c r="J164" s="21">
         <f>IF(F164 = "yes",G164, 0)</f>
@@ -8112,7 +8120,7 @@
       <c r="H172" s="11"/>
       <c r="I172" s="58">
         <f t="shared" ref="I172:K172" si="23">SUM(I4:I164)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J172" s="28">
         <f t="shared" si="23"/>

</xml_diff>

<commit_message>
1.6 Seed script to create 100 products across 4 categories
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8D6110DE-3FFF-4960-8F2E-61F438AE1089}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F1AB2060-A2A4-49C6-A107-884E0A0B9E54}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="9435" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1498,8 +1498,8 @@
   <dimension ref="A1:AC1121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D15" sqref="D15"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
2.1 Allow navigation of products through front page
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="26" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F1AB2060-A2A4-49C6-A107-884E0A0B9E54}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1AA08845-A4BA-4A4E-AEEE-B235764DD4CB}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="9435" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -873,7 +873,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1020,6 +1020,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1498,8 +1499,8 @@
   <dimension ref="A1:AC1121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D86" sqref="D86"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1516,7 +1517,7 @@
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; I172 &amp; "  /  Verified: " &amp; J172 &amp; "  /  Verified with Deductions: " &amp; K172 &amp; "  /  Verified with Deductions &amp; Milestones: " &amp; L172</f>
-        <v>Unverified Marks: 10  /  Verified: 0  /  Verified with Deductions: -30  /  Verified with Deductions &amp; Milestones: -30</v>
+        <v>Unverified Marks: 14  /  Verified: 0  /  Verified with Deductions: -30  /  Verified with Deductions &amp; Milestones: -30</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -2092,7 +2093,7 @@
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="25" t="s">
-        <v>20</v>
+        <v>216</v>
       </c>
       <c r="G15" s="26">
         <v>2</v>
@@ -2100,7 +2101,7 @@
       <c r="H15" s="27"/>
       <c r="I15" s="21">
         <f>IF(OR(F15 = "maybe", F15 = "yes"),G15, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J15" s="21">
         <f>IF(F15 = "yes",G15, 0)</f>
@@ -5631,7 +5632,7 @@
       </c>
       <c r="E107" s="11"/>
       <c r="F107" s="25" t="s">
-        <v>20</v>
+        <v>216</v>
       </c>
       <c r="G107" s="26">
         <v>2</v>
@@ -5641,7 +5642,7 @@
       </c>
       <c r="I107" s="21">
         <f>IF(OR(F107 = "maybe", F107 = "yes"),G107, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J107" s="21">
         <f>IF(F107 = "yes",G107, 0)</f>
@@ -5678,7 +5679,7 @@
         <v>142</v>
       </c>
       <c r="E108" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F108" s="30"/>
       <c r="G108" s="34"/>
@@ -5713,7 +5714,7 @@
         <v>143</v>
       </c>
       <c r="E109" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F109" s="30"/>
       <c r="G109" s="34"/>
@@ -5742,7 +5743,7 @@
     </row>
     <row r="110" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A110" s="8"/>
-      <c r="B110" s="8"/>
+      <c r="B110" s="60"/>
       <c r="C110" s="23" t="s">
         <v>144</v>
       </c>
@@ -8120,7 +8121,7 @@
       <c r="H172" s="11"/>
       <c r="I172" s="58">
         <f t="shared" ref="I172:K172" si="23">SUM(I4:I164)</f>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="J172" s="28">
         <f t="shared" si="23"/>

</xml_diff>

<commit_message>
2.5 Products listing are paginated
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1AA08845-A4BA-4A4E-AEEE-B235764DD4CB}"/>
+  <xr:revisionPtr revIDLastSave="61" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{428E384D-9C78-462D-8C50-9CB0CC262B98}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="9435" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="9150" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="383" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="218">
   <si>
     <t>Confirm</t>
   </si>
@@ -704,10 +704,10 @@
     <t>Yes Sum with Milestones</t>
   </si>
   <si>
-    <t>Maybe</t>
+    <t>33 // with 10% bonus</t>
   </si>
   <si>
-    <t>??</t>
+    <t>milestone 1</t>
   </si>
 </sst>
 </file>
@@ -1498,9 +1498,9 @@
   </sheetPr>
   <dimension ref="A1:AC1121"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H177" sqref="H177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1517,7 +1517,7 @@
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; I172 &amp; "  /  Verified: " &amp; J172 &amp; "  /  Verified with Deductions: " &amp; K172 &amp; "  /  Verified with Deductions &amp; Milestones: " &amp; L172</f>
-        <v>Unverified Marks: 14  /  Verified: 0  /  Verified with Deductions: -30  /  Verified with Deductions &amp; Milestones: -30</v>
+        <v>Unverified Marks: 30  /  Verified: 30  /  Verified with Deductions: 18  /  Verified with Deductions &amp; Milestones: 70</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -1641,7 +1641,7 @@
       </c>
       <c r="E4" s="11"/>
       <c r="F4" s="25" t="s">
-        <v>216</v>
+        <v>12</v>
       </c>
       <c r="G4" s="26">
         <v>2</v>
@@ -1655,11 +1655,11 @@
       </c>
       <c r="J4" s="28">
         <f t="shared" ref="J4:J5" si="1">IF(F4 = "yes",G4, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4" s="28">
         <f t="shared" ref="K4:K5" si="2">IF(F4 = "yes",G4, $M$2)</f>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="L4" s="22"/>
       <c r="M4" s="22"/>
@@ -1691,7 +1691,7 @@
       </c>
       <c r="E5" s="11"/>
       <c r="F5" s="25" t="s">
-        <v>216</v>
+        <v>12</v>
       </c>
       <c r="G5" s="26">
         <v>2</v>
@@ -1705,11 +1705,11 @@
       </c>
       <c r="J5" s="28">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K5" s="28">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="L5" s="22"/>
       <c r="M5" s="22"/>
@@ -1811,7 +1811,7 @@
       </c>
       <c r="E8" s="11"/>
       <c r="F8" s="25" t="s">
-        <v>216</v>
+        <v>12</v>
       </c>
       <c r="G8" s="26">
         <v>2</v>
@@ -1823,11 +1823,11 @@
       </c>
       <c r="J8" s="21">
         <f t="shared" ref="J8:J9" si="4">IF(F8 = "yes",G8, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K8" s="21">
         <f t="shared" ref="K8:K9" si="5">IF(F8 = "yes",G8, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L8" s="22"/>
       <c r="M8" s="22"/>
@@ -1859,7 +1859,7 @@
       </c>
       <c r="E9" s="11"/>
       <c r="F9" s="25" t="s">
-        <v>216</v>
+        <v>12</v>
       </c>
       <c r="G9" s="26">
         <v>2</v>
@@ -1871,11 +1871,11 @@
       </c>
       <c r="J9" s="21">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K9" s="21">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L9" s="22"/>
       <c r="M9" s="22"/>
@@ -2012,7 +2012,7 @@
       </c>
       <c r="E13" s="11"/>
       <c r="F13" s="25" t="s">
-        <v>216</v>
+        <v>12</v>
       </c>
       <c r="G13" s="26">
         <v>2</v>
@@ -2024,11 +2024,11 @@
       </c>
       <c r="J13" s="21">
         <f>IF(F13 = "yes",G13, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K13" s="21">
         <f>IF(F13 = "yes",G13, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L13" s="22"/>
       <c r="M13" s="22"/>
@@ -2093,7 +2093,7 @@
       </c>
       <c r="E15" s="11"/>
       <c r="F15" s="25" t="s">
-        <v>216</v>
+        <v>12</v>
       </c>
       <c r="G15" s="26">
         <v>2</v>
@@ -2105,11 +2105,11 @@
       </c>
       <c r="J15" s="21">
         <f>IF(F15 = "yes",G15, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K15" s="21">
         <f>IF(F15 = "yes",G15, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L15" s="22"/>
       <c r="M15" s="22"/>
@@ -2290,7 +2290,7 @@
       </c>
       <c r="E20" s="11"/>
       <c r="F20" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G20" s="26">
         <v>2</v>
@@ -2300,15 +2300,15 @@
       </c>
       <c r="I20" s="21">
         <f t="shared" ref="I20:I21" si="6">IF(OR(F20 = "maybe", F20 = "yes"),G20, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J20" s="21">
         <f t="shared" ref="J20:J21" si="7">IF(F20 = "yes",G20, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K20" s="21">
         <f>IF(F20 = "yes",G20, $M$2)</f>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="L20" s="22"/>
       <c r="M20" s="22"/>
@@ -2340,7 +2340,7 @@
       </c>
       <c r="E21" s="11"/>
       <c r="F21" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G21" s="26">
         <v>2</v>
@@ -2348,15 +2348,15 @@
       <c r="H21" s="32"/>
       <c r="I21" s="21">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J21" s="21">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K21" s="21">
         <f>IF(F21 = "yes",G21, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L21" s="22"/>
       <c r="M21" s="22"/>
@@ -2385,7 +2385,7 @@
         <v>40</v>
       </c>
       <c r="E22" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F22" s="30"/>
       <c r="G22" s="31"/>
@@ -2420,7 +2420,7 @@
         <v>41</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F23" s="30"/>
       <c r="G23" s="31"/>
@@ -2458,7 +2458,7 @@
       </c>
       <c r="E24" s="11"/>
       <c r="F24" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G24" s="26">
         <v>2</v>
@@ -2468,15 +2468,15 @@
       </c>
       <c r="I24" s="21">
         <f t="shared" ref="I24:I25" si="8">IF(OR(F24 = "maybe", F24 = "yes"),G24, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J24" s="21">
         <f t="shared" ref="J24:J25" si="9">IF(F24 = "yes",G24, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K24" s="21">
         <f>IF(F24 = "yes",G24, $M$2)</f>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="L24" s="22"/>
       <c r="M24" s="22"/>
@@ -5114,7 +5114,7 @@
     </row>
     <row r="94" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A94" s="8"/>
-      <c r="B94" s="8"/>
+      <c r="B94" s="60"/>
       <c r="C94" s="23" t="s">
         <v>125</v>
       </c>
@@ -5123,7 +5123,7 @@
       </c>
       <c r="E94" s="11"/>
       <c r="F94" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G94" s="26">
         <v>2</v>
@@ -5133,15 +5133,15 @@
       </c>
       <c r="I94" s="21">
         <f t="shared" ref="I94:I95" si="14">IF(OR(F94 = "maybe", F94 = "yes"),G94, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J94" s="21">
         <f t="shared" ref="J94:J95" si="15">IF(F94 = "yes",G94, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K94" s="21">
         <f>IF(F94 = "yes",G94, $M$2)</f>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="L94" s="22"/>
       <c r="M94" s="22"/>
@@ -5623,7 +5623,7 @@
     </row>
     <row r="107" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A107" s="8"/>
-      <c r="B107" s="8"/>
+      <c r="B107" s="60"/>
       <c r="C107" s="23" t="s">
         <v>140</v>
       </c>
@@ -5632,7 +5632,7 @@
       </c>
       <c r="E107" s="11"/>
       <c r="F107" s="25" t="s">
-        <v>216</v>
+        <v>12</v>
       </c>
       <c r="G107" s="26">
         <v>2</v>
@@ -5646,11 +5646,11 @@
       </c>
       <c r="J107" s="21">
         <f>IF(F107 = "yes",G107, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K107" s="21">
         <f>IF(F107 = "yes",G107, $M$2)</f>
-        <v>-3</v>
+        <v>2</v>
       </c>
       <c r="L107" s="22"/>
       <c r="M107" s="22"/>
@@ -6463,7 +6463,7 @@
     </row>
     <row r="128" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A128" s="8"/>
-      <c r="B128" s="8"/>
+      <c r="B128" s="60"/>
       <c r="C128" s="23" t="s">
         <v>167</v>
       </c>
@@ -6472,7 +6472,7 @@
       </c>
       <c r="E128" s="11"/>
       <c r="F128" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G128" s="26">
         <v>4</v>
@@ -6480,15 +6480,15 @@
       <c r="H128" s="32"/>
       <c r="I128" s="21">
         <f t="shared" ref="I128:I130" si="19">IF(OR(F128 = "maybe", F128 = "yes"),G128, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J128" s="21">
         <f t="shared" ref="J128:J130" si="20">IF(F128 = "yes",G128, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K128" s="21">
         <f t="shared" ref="K128:K130" si="21">IF(F128 = "yes",G128, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L128" s="22"/>
       <c r="M128" s="22"/>
@@ -7805,7 +7805,7 @@
     </row>
     <row r="164" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A164" s="8"/>
-      <c r="B164" s="8"/>
+      <c r="B164" s="60"/>
       <c r="C164" s="39" t="s">
         <v>204</v>
       </c>
@@ -7814,23 +7814,23 @@
       </c>
       <c r="E164" s="47"/>
       <c r="F164" s="25" t="s">
-        <v>216</v>
-      </c>
-      <c r="G164" s="46" t="s">
-        <v>217</v>
+        <v>12</v>
+      </c>
+      <c r="G164" s="46">
+        <v>4</v>
       </c>
       <c r="H164" s="32"/>
-      <c r="I164" s="21" t="str">
+      <c r="I164" s="21">
         <f>IF(OR(F164 = "maybe", F164 = "yes"),G164, 0)</f>
-        <v>??</v>
+        <v>4</v>
       </c>
       <c r="J164" s="21">
         <f>IF(F164 = "yes",G164, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K164" s="21">
         <f>IF(F164 = "yes",G164, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L164" s="22"/>
       <c r="M164" s="22"/>
@@ -7894,7 +7894,7 @@
         <v>207</v>
       </c>
       <c r="E166" s="54" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F166" s="20"/>
       <c r="G166" s="20"/>
@@ -7941,7 +7941,7 @@
       <c r="K167" s="21"/>
       <c r="L167" s="21">
         <f t="shared" ref="L167:L170" si="22">IF(E166="Yes", 1, 0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M167" s="22"/>
       <c r="N167" s="8"/>
@@ -8121,19 +8121,19 @@
       <c r="H172" s="11"/>
       <c r="I172" s="58">
         <f t="shared" ref="I172:K172" si="23">SUM(I4:I164)</f>
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="J172" s="28">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="K172" s="28">
         <f t="shared" si="23"/>
-        <v>-30</v>
+        <v>18</v>
       </c>
       <c r="L172" s="21">
         <f>CHOOSE(SUM(L167:L170)+1, MIN(60, K172) + (K172 - MIN(60, K172))/2,MIN(70, KJ172) + (K172 - MIN(70, K172))/2,MIN(80, K172) + (K172 - MIN(80, K172))/2,MIN(90, K172) + (K172 - MIN(90, K172))/2, K172)</f>
-        <v>-30</v>
+        <v>70</v>
       </c>
       <c r="M172" s="22"/>
       <c r="N172" s="8"/>
@@ -8160,9 +8160,13 @@
       <c r="D173" s="55"/>
       <c r="E173" s="8"/>
       <c r="F173" s="8"/>
-      <c r="G173" s="53"/>
+      <c r="G173" s="53" t="s">
+        <v>217</v>
+      </c>
       <c r="H173" s="8"/>
-      <c r="I173" s="53"/>
+      <c r="I173" s="53" t="s">
+        <v>216</v>
+      </c>
       <c r="J173" s="53"/>
       <c r="K173" s="53"/>
       <c r="L173" s="8"/>

</xml_diff>

<commit_message>
Add pagination to categories search
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="61" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{428E384D-9C78-462D-8C50-9CB0CC262B98}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{852086DD-2B36-4AA3-9B32-D91DFA3C4B04}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9150" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="219">
   <si>
     <t>Confirm</t>
   </si>
@@ -709,6 +709,9 @@
   <si>
     <t>milestone 1</t>
   </si>
+  <si>
+    <t>Maybe</t>
+  </si>
 </sst>
 </file>
 
@@ -873,7 +876,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1021,6 +1024,8 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1499,8 +1504,8 @@
   <dimension ref="A1:AC1121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A158" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H177" sqref="H177"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1517,7 +1522,7 @@
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; I172 &amp; "  /  Verified: " &amp; J172 &amp; "  /  Verified with Deductions: " &amp; K172 &amp; "  /  Verified with Deductions &amp; Milestones: " &amp; L172</f>
-        <v>Unverified Marks: 30  /  Verified: 30  /  Verified with Deductions: 18  /  Verified with Deductions &amp; Milestones: 70</v>
+        <v>Unverified Marks: 32  /  Verified: 30  /  Verified with Deductions: 18  /  Verified with Deductions &amp; Milestones: 70</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -1632,7 +1637,7 @@
     </row>
     <row r="4" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
-      <c r="B4" s="59"/>
+      <c r="B4" s="61"/>
       <c r="C4" s="23" t="s">
         <v>10</v>
       </c>
@@ -1682,7 +1687,7 @@
     </row>
     <row r="5" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
-      <c r="B5" s="59"/>
+      <c r="B5" s="61"/>
       <c r="C5" s="23" t="s">
         <v>14</v>
       </c>
@@ -1732,7 +1737,7 @@
     </row>
     <row r="6" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
-      <c r="B6" s="10"/>
+      <c r="B6" s="61"/>
       <c r="C6" s="23"/>
       <c r="D6" s="29" t="s">
         <v>16</v>
@@ -1767,7 +1772,7 @@
     </row>
     <row r="7" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
+      <c r="B7" s="61"/>
       <c r="C7" s="23"/>
       <c r="D7" s="29" t="s">
         <v>17</v>
@@ -1802,7 +1807,7 @@
     </row>
     <row r="8" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
-      <c r="B8" s="59"/>
+      <c r="B8" s="61"/>
       <c r="C8" s="23" t="s">
         <v>18</v>
       </c>
@@ -1850,7 +1855,7 @@
     </row>
     <row r="9" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
-      <c r="B9" s="59"/>
+      <c r="B9" s="61"/>
       <c r="C9" s="23" t="s">
         <v>21</v>
       </c>
@@ -2003,7 +2008,7 @@
     </row>
     <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
-      <c r="B13" s="59"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="23" t="s">
         <v>26</v>
       </c>
@@ -2051,7 +2056,7 @@
     </row>
     <row r="14" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="62" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="23"/>
@@ -2084,7 +2089,7 @@
     </row>
     <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
-      <c r="B15" s="59"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="23" t="s">
         <v>29</v>
       </c>
@@ -2281,7 +2286,7 @@
     </row>
     <row r="20" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
-      <c r="B20" s="59"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="23" t="s">
         <v>36</v>
       </c>
@@ -2331,7 +2336,7 @@
     </row>
     <row r="21" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
-      <c r="B21" s="59"/>
+      <c r="B21" s="61"/>
       <c r="C21" s="23" t="s">
         <v>38</v>
       </c>
@@ -2449,7 +2454,7 @@
     </row>
     <row r="24" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
-      <c r="B24" s="59"/>
+      <c r="B24" s="61"/>
       <c r="C24" s="23" t="s">
         <v>42</v>
       </c>
@@ -2696,7 +2701,7 @@
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="25" t="s">
-        <v>20</v>
+        <v>218</v>
       </c>
       <c r="G30" s="26">
         <v>2</v>
@@ -2704,7 +2709,7 @@
       <c r="H30" s="32"/>
       <c r="I30" s="21">
         <f t="shared" ref="I30:I31" si="10">IF(OR(F30 = "maybe", F30 = "yes"),G30, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J30" s="21">
         <f t="shared" ref="J30:J31" si="11">IF(F30 = "yes",G30, 0)</f>
@@ -8121,7 +8126,7 @@
       <c r="H172" s="11"/>
       <c r="I172" s="58">
         <f t="shared" ref="I172:K172" si="23">SUM(I4:I164)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="J172" s="28">
         <f t="shared" si="23"/>

</xml_diff>

<commit_message>
2.6 Search through the avaliable products using keyword search by category
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="67" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{852086DD-2B36-4AA3-9B32-D91DFA3C4B04}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D730D6D3-9040-477F-884E-BE545183EA5E}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9150" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1505,7 +1505,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F30" sqref="F30"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1522,7 +1522,7 @@
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; I172 &amp; "  /  Verified: " &amp; J172 &amp; "  /  Verified with Deductions: " &amp; K172 &amp; "  /  Verified with Deductions &amp; Milestones: " &amp; L172</f>
-        <v>Unverified Marks: 32  /  Verified: 30  /  Verified with Deductions: 18  /  Verified with Deductions &amp; Milestones: 70</v>
+        <v>Unverified Marks: 36  /  Verified: 30  /  Verified with Deductions: 18  /  Verified with Deductions &amp; Milestones: 70</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -2749,7 +2749,7 @@
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="25" t="s">
-        <v>20</v>
+        <v>218</v>
       </c>
       <c r="G31" s="26">
         <v>4</v>
@@ -2759,7 +2759,7 @@
       </c>
       <c r="I31" s="21">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J31" s="21">
         <f t="shared" si="11"/>
@@ -2796,7 +2796,7 @@
         <v>54</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F32" s="30"/>
       <c r="G32" s="31"/>
@@ -2831,7 +2831,7 @@
         <v>55</v>
       </c>
       <c r="E33" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F33" s="30"/>
       <c r="G33" s="31"/>
@@ -2866,7 +2866,7 @@
         <v>56</v>
       </c>
       <c r="E34" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F34" s="30"/>
       <c r="G34" s="31"/>
@@ -2901,7 +2901,7 @@
         <v>57</v>
       </c>
       <c r="E35" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F35" s="30"/>
       <c r="G35" s="31"/>
@@ -2936,7 +2936,7 @@
         <v>58</v>
       </c>
       <c r="E36" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F36" s="30"/>
       <c r="G36" s="31"/>
@@ -2971,7 +2971,7 @@
         <v>59</v>
       </c>
       <c r="E37" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F37" s="30"/>
       <c r="G37" s="31"/>
@@ -8126,7 +8126,7 @@
       <c r="H172" s="11"/>
       <c r="I172" s="58">
         <f t="shared" ref="I172:K172" si="23">SUM(I4:I164)</f>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="J172" s="28">
         <f t="shared" si="23"/>

</xml_diff>

<commit_message>
fix issue where active admin set images in active admin were not updating. And minor styling changes on new product search checkbox
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D730D6D3-9040-477F-884E-BE545183EA5E}"/>
+  <xr:revisionPtr revIDLastSave="120" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7DBA4863-7B71-4F33-A2F9-E987FAA88C93}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9150" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="220">
   <si>
     <t>Confirm</t>
   </si>
@@ -710,7 +710,10 @@
     <t>milestone 1</t>
   </si>
   <si>
-    <t>Maybe</t>
+    <t>46//with 10%</t>
+  </si>
+  <si>
+    <t>milestone 2</t>
   </si>
 </sst>
 </file>
@@ -844,7 +847,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1022,10 +1025,10 @@
     <xf numFmtId="1" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1504,8 +1507,8 @@
   <dimension ref="A1:AC1121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1513,7 +1516,7 @@
     <col min="1" max="1" width="4.85546875" customWidth="1"/>
     <col min="2" max="2" width="7" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" customWidth="1"/>
-    <col min="4" max="4" width="149.28515625" customWidth="1"/>
+    <col min="4" max="4" width="155" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" customWidth="1"/>
     <col min="11" max="11" width="28.28515625" customWidth="1"/>
     <col min="12" max="12" width="28.7109375" customWidth="1"/>
@@ -1522,7 +1525,7 @@
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; I172 &amp; "  /  Verified: " &amp; J172 &amp; "  /  Verified with Deductions: " &amp; K172 &amp; "  /  Verified with Deductions &amp; Milestones: " &amp; L172</f>
-        <v>Unverified Marks: 36  /  Verified: 30  /  Verified with Deductions: 18  /  Verified with Deductions &amp; Milestones: 70</v>
+        <v>Unverified Marks: 42  /  Verified: 42  /  Verified with Deductions: 36  /  Verified with Deductions &amp; Milestones: 70</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -1637,7 +1640,7 @@
     </row>
     <row r="4" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A4" s="10"/>
-      <c r="B4" s="61"/>
+      <c r="B4" s="59"/>
       <c r="C4" s="23" t="s">
         <v>10</v>
       </c>
@@ -1687,7 +1690,7 @@
     </row>
     <row r="5" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="10"/>
-      <c r="B5" s="61"/>
+      <c r="B5" s="59"/>
       <c r="C5" s="23" t="s">
         <v>14</v>
       </c>
@@ -1737,7 +1740,7 @@
     </row>
     <row r="6" spans="1:29" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10"/>
-      <c r="B6" s="61"/>
+      <c r="B6" s="59"/>
       <c r="C6" s="23"/>
       <c r="D6" s="29" t="s">
         <v>16</v>
@@ -1772,7 +1775,7 @@
     </row>
     <row r="7" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
-      <c r="B7" s="61"/>
+      <c r="B7" s="59"/>
       <c r="C7" s="23"/>
       <c r="D7" s="29" t="s">
         <v>17</v>
@@ -1807,7 +1810,7 @@
     </row>
     <row r="8" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A8" s="10"/>
-      <c r="B8" s="61"/>
+      <c r="B8" s="59"/>
       <c r="C8" s="23" t="s">
         <v>18</v>
       </c>
@@ -1855,7 +1858,7 @@
     </row>
     <row r="9" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A9" s="10"/>
-      <c r="B9" s="61"/>
+      <c r="B9" s="59"/>
       <c r="C9" s="23" t="s">
         <v>21</v>
       </c>
@@ -2008,7 +2011,7 @@
     </row>
     <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A13" s="10"/>
-      <c r="B13" s="61"/>
+      <c r="B13" s="59"/>
       <c r="C13" s="23" t="s">
         <v>26</v>
       </c>
@@ -2056,7 +2059,7 @@
     </row>
     <row r="14" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A14" s="17"/>
-      <c r="B14" s="62" t="s">
+      <c r="B14" s="60" t="s">
         <v>28</v>
       </c>
       <c r="C14" s="23"/>
@@ -2089,7 +2092,7 @@
     </row>
     <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
-      <c r="B15" s="61"/>
+      <c r="B15" s="59"/>
       <c r="C15" s="23" t="s">
         <v>29</v>
       </c>
@@ -2286,7 +2289,7 @@
     </row>
     <row r="20" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A20" s="10"/>
-      <c r="B20" s="61"/>
+      <c r="B20" s="59"/>
       <c r="C20" s="23" t="s">
         <v>36</v>
       </c>
@@ -2336,7 +2339,7 @@
     </row>
     <row r="21" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A21" s="10"/>
-      <c r="B21" s="61"/>
+      <c r="B21" s="59"/>
       <c r="C21" s="23" t="s">
         <v>38</v>
       </c>
@@ -2454,7 +2457,7 @@
     </row>
     <row r="24" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
-      <c r="B24" s="61"/>
+      <c r="B24" s="59"/>
       <c r="C24" s="23" t="s">
         <v>42</v>
       </c>
@@ -2513,7 +2516,7 @@
       </c>
       <c r="E25" s="11"/>
       <c r="F25" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G25" s="26">
         <v>2</v>
@@ -2521,15 +2524,15 @@
       <c r="H25" s="32"/>
       <c r="I25" s="21">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J25" s="21">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K25" s="21">
         <f>IF(F25 = "yes",G25, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L25" s="22"/>
       <c r="M25" s="22"/>
@@ -2558,7 +2561,7 @@
         <v>46</v>
       </c>
       <c r="E26" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F26" s="30"/>
       <c r="G26" s="31"/>
@@ -2593,7 +2596,7 @@
         <v>47</v>
       </c>
       <c r="E27" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F27" s="30"/>
       <c r="G27" s="31"/>
@@ -2620,7 +2623,7 @@
       <c r="AB27" s="8"/>
       <c r="AC27" s="8"/>
     </row>
-    <row r="28" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A28" s="10"/>
       <c r="B28" s="10"/>
       <c r="C28" s="23"/>
@@ -2628,7 +2631,7 @@
         <v>48</v>
       </c>
       <c r="E28" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F28" s="30"/>
       <c r="G28" s="31"/>
@@ -2663,7 +2666,7 @@
         <v>49</v>
       </c>
       <c r="E29" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F29" s="30"/>
       <c r="G29" s="31"/>
@@ -2701,7 +2704,7 @@
       </c>
       <c r="E30" s="11"/>
       <c r="F30" s="25" t="s">
-        <v>218</v>
+        <v>12</v>
       </c>
       <c r="G30" s="26">
         <v>2</v>
@@ -2713,11 +2716,11 @@
       </c>
       <c r="J30" s="21">
         <f t="shared" ref="J30:J31" si="11">IF(F30 = "yes",G30, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K30" s="21">
         <f>IF(F30 = "yes",G30, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="L30" s="22"/>
       <c r="M30" s="22"/>
@@ -2749,7 +2752,7 @@
       </c>
       <c r="E31" s="11"/>
       <c r="F31" s="25" t="s">
-        <v>218</v>
+        <v>12</v>
       </c>
       <c r="G31" s="26">
         <v>4</v>
@@ -2763,11 +2766,11 @@
       </c>
       <c r="J31" s="21">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K31" s="21">
         <f>IF(F31 = "yes",G31, $M$2)</f>
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="L31" s="22"/>
       <c r="M31" s="22"/>
@@ -3066,7 +3069,7 @@
     </row>
     <row r="40" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
+      <c r="B40" s="62"/>
       <c r="C40" s="23" t="s">
         <v>61</v>
       </c>
@@ -3075,7 +3078,7 @@
       </c>
       <c r="E40" s="11"/>
       <c r="F40" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G40" s="26">
         <v>4</v>
@@ -3085,15 +3088,15 @@
       </c>
       <c r="I40" s="21">
         <f t="shared" ref="I40:I41" si="12">IF(OR(F40 = "maybe", F40 = "yes"),G40, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J40" s="21">
         <f t="shared" ref="J40:J41" si="13">IF(F40 = "yes",G40, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K40" s="21">
         <f>IF(F40 = "yes",G40, $M$2)</f>
-        <v>-3</v>
+        <v>4</v>
       </c>
       <c r="L40" s="22"/>
       <c r="M40" s="22"/>
@@ -3116,7 +3119,7 @@
     </row>
     <row r="41" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
+      <c r="B41" s="61"/>
       <c r="C41" s="23" t="s">
         <v>63</v>
       </c>
@@ -3268,7 +3271,7 @@
     </row>
     <row r="45" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
+      <c r="B45" s="61"/>
       <c r="C45" s="23" t="s">
         <v>68</v>
       </c>
@@ -3493,7 +3496,7 @@
     </row>
     <row r="51" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
+      <c r="B51" s="61"/>
       <c r="C51" s="23" t="s">
         <v>75</v>
       </c>
@@ -3681,7 +3684,7 @@
     </row>
     <row r="56" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
+      <c r="B56" s="61"/>
       <c r="C56" s="39" t="s">
         <v>81</v>
       </c>
@@ -4206,7 +4209,7 @@
     </row>
     <row r="70" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A70" s="8"/>
-      <c r="B70" s="8"/>
+      <c r="B70" s="61"/>
       <c r="C70" s="23" t="s">
         <v>98</v>
       </c>
@@ -4357,7 +4360,7 @@
     </row>
     <row r="74" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A74" s="8"/>
-      <c r="B74" s="8"/>
+      <c r="B74" s="61"/>
       <c r="C74" s="23" t="s">
         <v>102</v>
       </c>
@@ -4545,7 +4548,7 @@
     </row>
     <row r="79" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A79" s="8"/>
-      <c r="B79" s="8"/>
+      <c r="B79" s="61"/>
       <c r="C79" s="23" t="s">
         <v>108</v>
       </c>
@@ -4591,9 +4594,9 @@
       <c r="AB79" s="8"/>
       <c r="AC79" s="8"/>
     </row>
-    <row r="80" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A80" s="8"/>
-      <c r="B80" s="8"/>
+      <c r="B80" s="62"/>
       <c r="C80" s="23"/>
       <c r="D80" s="29" t="s">
         <v>110</v>
@@ -5119,7 +5122,7 @@
     </row>
     <row r="94" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A94" s="8"/>
-      <c r="B94" s="60"/>
+      <c r="B94" s="62"/>
       <c r="C94" s="23" t="s">
         <v>125</v>
       </c>
@@ -5341,7 +5344,7 @@
         <v>132</v>
       </c>
       <c r="E99" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F99" s="30"/>
       <c r="G99" s="34"/>
@@ -5376,7 +5379,7 @@
         <v>133</v>
       </c>
       <c r="E100" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F100" s="30"/>
       <c r="G100" s="34"/>
@@ -5628,7 +5631,7 @@
     </row>
     <row r="107" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A107" s="8"/>
-      <c r="B107" s="60"/>
+      <c r="B107" s="62"/>
       <c r="C107" s="23" t="s">
         <v>140</v>
       </c>
@@ -5748,7 +5751,7 @@
     </row>
     <row r="110" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A110" s="8"/>
-      <c r="B110" s="60"/>
+      <c r="B110" s="61"/>
       <c r="C110" s="23" t="s">
         <v>144</v>
       </c>
@@ -6468,7 +6471,7 @@
     </row>
     <row r="128" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A128" s="8"/>
-      <c r="B128" s="60"/>
+      <c r="B128" s="62"/>
       <c r="C128" s="23" t="s">
         <v>167</v>
       </c>
@@ -7009,7 +7012,7 @@
       <c r="AB141" s="8"/>
       <c r="AC141" s="8"/>
     </row>
-    <row r="142" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A142" s="8"/>
       <c r="B142" s="8"/>
       <c r="C142" s="23"/>
@@ -7162,7 +7165,7 @@
       <c r="AB145" s="8"/>
       <c r="AC145" s="8"/>
     </row>
-    <row r="146" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A146" s="8"/>
       <c r="B146" s="8"/>
       <c r="C146" s="23"/>
@@ -7315,7 +7318,7 @@
       <c r="AB149" s="8"/>
       <c r="AC149" s="8"/>
     </row>
-    <row r="150" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A150" s="8"/>
       <c r="B150" s="8"/>
       <c r="C150" s="23"/>
@@ -7385,7 +7388,7 @@
       <c r="AB151" s="8"/>
       <c r="AC151" s="8"/>
     </row>
-    <row r="152" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A152" s="8"/>
       <c r="B152" s="8"/>
       <c r="C152" s="23"/>
@@ -7810,7 +7813,7 @@
     </row>
     <row r="164" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A164" s="8"/>
-      <c r="B164" s="60"/>
+      <c r="B164" s="62"/>
       <c r="C164" s="39" t="s">
         <v>204</v>
       </c>
@@ -8126,15 +8129,15 @@
       <c r="H172" s="11"/>
       <c r="I172" s="58">
         <f t="shared" ref="I172:K172" si="23">SUM(I4:I164)</f>
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="J172" s="28">
         <f t="shared" si="23"/>
-        <v>30</v>
+        <v>42</v>
       </c>
       <c r="K172" s="28">
         <f t="shared" si="23"/>
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="L172" s="21">
         <f>CHOOSE(SUM(L167:L170)+1, MIN(60, K172) + (K172 - MIN(60, K172))/2,MIN(70, KJ172) + (K172 - MIN(70, K172))/2,MIN(80, K172) + (K172 - MIN(80, K172))/2,MIN(90, K172) + (K172 - MIN(90, K172))/2, K172)</f>
@@ -8200,8 +8203,12 @@
       <c r="D174" s="55"/>
       <c r="E174" s="8"/>
       <c r="F174" s="8"/>
-      <c r="G174" s="53"/>
-      <c r="H174" s="8"/>
+      <c r="G174" s="53" t="s">
+        <v>219</v>
+      </c>
+      <c r="H174" s="8" t="s">
+        <v>218</v>
+      </c>
       <c r="I174" s="53"/>
       <c r="J174" s="53"/>
       <c r="K174" s="53"/>

</xml_diff>

<commit_message>
3.3.1 Add stripe gem and associated js
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="8_{7E8DBD90-0D90-4670-8C6F-3EFA8D5AB8DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7DBA4863-7B71-4F33-A2F9-E987FAA88C93}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="109_{1E4BBE9D-18EA-49A5-9CF1-0233A02ADE58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{21FAC918-69DB-4CD1-9339-53595A26A36C}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9150" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="221">
   <si>
     <t>Confirm</t>
   </si>
@@ -715,6 +715,9 @@
   <si>
     <t>milestone 2</t>
   </si>
+  <si>
+    <t>Maybe</t>
+  </si>
 </sst>
 </file>
 
@@ -826,7 +829,7 @@
       <name val="Consolas"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -848,6 +851,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -879,7 +888,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1029,6 +1038,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1507,8 +1517,8 @@
   <dimension ref="A1:AC1121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B40" sqref="B40"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1525,7 +1535,7 @@
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; I172 &amp; "  /  Verified: " &amp; J172 &amp; "  /  Verified with Deductions: " &amp; K172 &amp; "  /  Verified with Deductions &amp; Milestones: " &amp; L172</f>
-        <v>Unverified Marks: 42  /  Verified: 42  /  Verified with Deductions: 36  /  Verified with Deductions &amp; Milestones: 70</v>
+        <v>Unverified Marks: 46  /  Verified: 42  /  Verified with Deductions: 36  /  Verified with Deductions &amp; Milestones: 70</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -3128,7 +3138,7 @@
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="25" t="s">
-        <v>20</v>
+        <v>220</v>
       </c>
       <c r="G41" s="26">
         <v>4</v>
@@ -3136,7 +3146,7 @@
       <c r="H41" s="32"/>
       <c r="I41" s="21">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J41" s="21">
         <f t="shared" si="13"/>
@@ -3172,7 +3182,7 @@
         <v>65</v>
       </c>
       <c r="E42" s="37" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F42" s="30"/>
       <c r="G42" s="34"/>
@@ -3207,7 +3217,7 @@
         <v>66</v>
       </c>
       <c r="E43" s="37" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F43" s="30"/>
       <c r="G43" s="34"/>
@@ -3242,7 +3252,7 @@
         <v>67</v>
       </c>
       <c r="E44" s="37" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F44" s="30"/>
       <c r="G44" s="34"/>
@@ -3270,7 +3280,7 @@
       <c r="AC44" s="8"/>
     </row>
     <row r="45" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="8"/>
+      <c r="A45" s="63"/>
       <c r="B45" s="61"/>
       <c r="C45" s="23" t="s">
         <v>68</v>
@@ -4359,7 +4369,7 @@
       <c r="AC73" s="8"/>
     </row>
     <row r="74" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="8"/>
+      <c r="A74" s="63"/>
       <c r="B74" s="61"/>
       <c r="C74" s="23" t="s">
         <v>102</v>
@@ -8129,7 +8139,7 @@
       <c r="H172" s="11"/>
       <c r="I172" s="58">
         <f t="shared" ref="I172:K172" si="23">SUM(I4:I164)</f>
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="J172" s="28">
         <f t="shared" si="23"/>

</xml_diff>

<commit_message>
3.1.4 Added users using devise
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="109_{1E4BBE9D-18EA-49A5-9CF1-0233A02ADE58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{21FAC918-69DB-4CD1-9339-53595A26A36C}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="109_{21EAC73E-584B-4B3F-8E40-DD04FB917DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F2FFA663-9B8E-4982-84E1-E388707C96DD}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9150" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1518,7 +1518,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D74" sqref="D74"/>
+      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3595,7 +3595,7 @@
         <v>78</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F53" s="30"/>
       <c r="G53" s="34"/>
@@ -3665,7 +3665,7 @@
         <v>80</v>
       </c>
       <c r="E55" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F55" s="30"/>
       <c r="G55" s="34"/>

</xml_diff>

<commit_message>
Added Provinces and taxes to database
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="109_{21EAC73E-584B-4B3F-8E40-DD04FB917DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{F2FFA663-9B8E-4982-84E1-E388707C96DD}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="109_{21EAC73E-584B-4B3F-8E40-DD04FB917DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D7C57A47-D71C-4A4A-AD86-55F592F19AD6}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9150" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1517,8 +1517,8 @@
   <dimension ref="A1:AC1121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1535,7 +1535,7 @@
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; I172 &amp; "  /  Verified: " &amp; J172 &amp; "  /  Verified with Deductions: " &amp; K172 &amp; "  /  Verified with Deductions &amp; Milestones: " &amp; L172</f>
-        <v>Unverified Marks: 46  /  Verified: 42  /  Verified with Deductions: 36  /  Verified with Deductions &amp; Milestones: 70</v>
+        <v>Unverified Marks: 54  /  Verified: 42  /  Verified with Deductions: 36  /  Verified with Deductions &amp; Milestones: 70</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -3515,7 +3515,7 @@
       </c>
       <c r="E51" s="11"/>
       <c r="F51" s="25" t="s">
-        <v>20</v>
+        <v>220</v>
       </c>
       <c r="G51" s="26">
         <v>8</v>
@@ -3523,7 +3523,7 @@
       <c r="H51" s="32"/>
       <c r="I51" s="21">
         <f>IF(OR(F51 = "maybe", F51 = "yes"),G51, 0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J51" s="21">
         <f>IF(F51 = "yes",G51, 0)</f>
@@ -3560,7 +3560,7 @@
         <v>77</v>
       </c>
       <c r="E52" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F52" s="30"/>
       <c r="G52" s="34"/>
@@ -3630,7 +3630,7 @@
         <v>79</v>
       </c>
       <c r="E54" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F54" s="30"/>
       <c r="G54" s="34"/>
@@ -4424,7 +4424,7 @@
         <v>104</v>
       </c>
       <c r="E75" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F75" s="30"/>
       <c r="G75" s="34"/>
@@ -4459,7 +4459,7 @@
         <v>105</v>
       </c>
       <c r="E76" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F76" s="30"/>
       <c r="G76" s="34"/>
@@ -4529,7 +4529,7 @@
         <v>107</v>
       </c>
       <c r="E78" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F78" s="30"/>
       <c r="G78" s="34"/>
@@ -8139,7 +8139,7 @@
       <c r="H172" s="11"/>
       <c r="I172" s="58">
         <f t="shared" ref="I172:K172" si="23">SUM(I4:I164)</f>
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="J172" s="28">
         <f t="shared" si="23"/>

</xml_diff>

<commit_message>
3.1.5 Add Province to user and allow user to edit their province
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="109_{21EAC73E-584B-4B3F-8E40-DD04FB917DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D7C57A47-D71C-4A4A-AD86-55F592F19AD6}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="109_{21EAC73E-584B-4B3F-8E40-DD04FB917DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C578D989-3ECE-44AE-AED9-4B965D2FD9A9}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="9150" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1517,8 +1517,8 @@
   <dimension ref="A1:AC1121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D49" sqref="D49"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -6256,7 +6256,7 @@
     </row>
     <row r="122" spans="1:29" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A122" s="8"/>
-      <c r="B122" s="8"/>
+      <c r="B122" s="61"/>
       <c r="C122" s="23" t="s">
         <v>160</v>
       </c>
@@ -6312,7 +6312,7 @@
         <v>162</v>
       </c>
       <c r="E123" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F123" s="30"/>
       <c r="G123" s="34"/>
@@ -6382,7 +6382,7 @@
         <v>164</v>
       </c>
       <c r="E125" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F125" s="30"/>
       <c r="G125" s="34"/>
@@ -6417,7 +6417,7 @@
         <v>165</v>
       </c>
       <c r="E126" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F126" s="30"/>
       <c r="G126" s="34"/>
@@ -6452,7 +6452,7 @@
         <v>166</v>
       </c>
       <c r="E127" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F127" s="30"/>
       <c r="G127" s="34"/>

</xml_diff>

<commit_message>
3.1.3 Add route to checkout invoice
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="109_{21EAC73E-584B-4B3F-8E40-DD04FB917DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{C578D989-3ECE-44AE-AED9-4B965D2FD9A9}"/>
+  <xr:revisionPtr revIDLastSave="39" documentId="109_{21EAC73E-584B-4B3F-8E40-DD04FB917DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{565BE605-A534-4FA3-A16F-FB402F19B849}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9150" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28800" yWindow="9270" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="222">
   <si>
     <t>Confirm</t>
   </si>
@@ -716,7 +716,10 @@
     <t>milestone 2</t>
   </si>
   <si>
-    <t>Maybe</t>
+    <t>milestone 3</t>
+  </si>
+  <si>
+    <t>62 // with 10%</t>
   </si>
 </sst>
 </file>
@@ -829,7 +832,7 @@
       <name val="Consolas"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -851,12 +854,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -888,7 +885,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1038,7 +1035,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1517,8 +1513,8 @@
   <dimension ref="A1:AC1121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1535,7 +1531,7 @@
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; I172 &amp; "  /  Verified: " &amp; J172 &amp; "  /  Verified with Deductions: " &amp; K172 &amp; "  /  Verified with Deductions &amp; Milestones: " &amp; L172</f>
-        <v>Unverified Marks: 54  /  Verified: 42  /  Verified with Deductions: 36  /  Verified with Deductions &amp; Milestones: 70</v>
+        <v>Unverified Marks: 58  /  Verified: 58  /  Verified with Deductions: 52  /  Verified with Deductions &amp; Milestones: 70</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -3128,8 +3124,8 @@
       <c r="AC40" s="8"/>
     </row>
     <row r="41" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A41" s="8"/>
-      <c r="B41" s="61"/>
+      <c r="A41" s="62"/>
+      <c r="B41" s="62"/>
       <c r="C41" s="23" t="s">
         <v>63</v>
       </c>
@@ -3138,7 +3134,7 @@
       </c>
       <c r="E41" s="11"/>
       <c r="F41" s="25" t="s">
-        <v>220</v>
+        <v>12</v>
       </c>
       <c r="G41" s="26">
         <v>4</v>
@@ -3150,11 +3146,11 @@
       </c>
       <c r="J41" s="21">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K41" s="21">
         <f>IF(F41 = "yes",G41, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L41" s="22"/>
       <c r="M41" s="22"/>
@@ -3280,7 +3276,7 @@
       <c r="AC44" s="8"/>
     </row>
     <row r="45" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A45" s="63"/>
+      <c r="A45" s="62"/>
       <c r="B45" s="61"/>
       <c r="C45" s="23" t="s">
         <v>68</v>
@@ -3407,7 +3403,7 @@
         <v>72</v>
       </c>
       <c r="E48" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F48" s="30"/>
       <c r="G48" s="34"/>
@@ -3505,8 +3501,8 @@
       <c r="AC50" s="8"/>
     </row>
     <row r="51" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A51" s="8"/>
-      <c r="B51" s="61"/>
+      <c r="A51" s="62"/>
+      <c r="B51" s="62"/>
       <c r="C51" s="23" t="s">
         <v>75</v>
       </c>
@@ -3515,7 +3511,7 @@
       </c>
       <c r="E51" s="11"/>
       <c r="F51" s="25" t="s">
-        <v>220</v>
+        <v>12</v>
       </c>
       <c r="G51" s="26">
         <v>8</v>
@@ -3527,11 +3523,11 @@
       </c>
       <c r="J51" s="21">
         <f>IF(F51 = "yes",G51, 0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="K51" s="21">
         <f>IF(F51 = "yes",G51, 0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L51" s="22"/>
       <c r="M51" s="22"/>
@@ -3693,8 +3689,8 @@
       <c r="AC55" s="8"/>
     </row>
     <row r="56" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A56" s="8"/>
-      <c r="B56" s="61"/>
+      <c r="A56" s="62"/>
+      <c r="B56" s="62"/>
       <c r="C56" s="39" t="s">
         <v>81</v>
       </c>
@@ -3703,7 +3699,7 @@
       </c>
       <c r="E56" s="11"/>
       <c r="F56" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="G56" s="26">
         <v>4</v>
@@ -3711,15 +3707,15 @@
       <c r="H56" s="32"/>
       <c r="I56" s="21">
         <f>IF(OR(F56 = "maybe", F56 = "yes"),G56, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J56" s="21">
         <f>IF(F56 = "yes",G56, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K56" s="21">
         <f>IF(F56 = "yes",G56, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="L56" s="22"/>
       <c r="M56" s="22"/>
@@ -3748,7 +3744,7 @@
         <v>83</v>
       </c>
       <c r="E57" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F57" s="30"/>
       <c r="G57" s="30"/>
@@ -3783,7 +3779,7 @@
         <v>84</v>
       </c>
       <c r="E58" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F58" s="30"/>
       <c r="G58" s="30"/>
@@ -4218,7 +4214,7 @@
       <c r="AC69" s="8"/>
     </row>
     <row r="70" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A70" s="8"/>
+      <c r="A70" s="62"/>
       <c r="B70" s="61"/>
       <c r="C70" s="23" t="s">
         <v>98</v>
@@ -4308,7 +4304,7 @@
         <v>101</v>
       </c>
       <c r="E72" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F72" s="30"/>
       <c r="G72" s="34"/>
@@ -4369,7 +4365,7 @@
       <c r="AC73" s="8"/>
     </row>
     <row r="74" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A74" s="63"/>
+      <c r="A74" s="62"/>
       <c r="B74" s="61"/>
       <c r="C74" s="23" t="s">
         <v>102</v>
@@ -8139,15 +8135,15 @@
       <c r="H172" s="11"/>
       <c r="I172" s="58">
         <f t="shared" ref="I172:K172" si="23">SUM(I4:I164)</f>
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="J172" s="28">
         <f t="shared" si="23"/>
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="K172" s="28">
         <f t="shared" si="23"/>
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="L172" s="21">
         <f>CHOOSE(SUM(L167:L170)+1, MIN(60, K172) + (K172 - MIN(60, K172))/2,MIN(70, KJ172) + (K172 - MIN(70, K172))/2,MIN(80, K172) + (K172 - MIN(80, K172))/2,MIN(90, K172) + (K172 - MIN(90, K172))/2, K172)</f>
@@ -8248,8 +8244,12 @@
       <c r="D175" s="55"/>
       <c r="E175" s="8"/>
       <c r="F175" s="8"/>
-      <c r="G175" s="53"/>
-      <c r="H175" s="8"/>
+      <c r="G175" s="53" t="s">
+        <v>220</v>
+      </c>
+      <c r="H175" s="8" t="s">
+        <v>221</v>
+      </c>
       <c r="I175" s="53"/>
       <c r="J175" s="53"/>
       <c r="K175" s="53"/>

</xml_diff>

<commit_message>
3.1.3 Display invoice to customer
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="39" documentId="109_{21EAC73E-584B-4B3F-8E40-DD04FB917DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{565BE605-A534-4FA3-A16F-FB402F19B849}"/>
+  <xr:revisionPtr revIDLastSave="40" documentId="109_{21EAC73E-584B-4B3F-8E40-DD04FB917DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7CE1B172-6143-4AD6-9A8F-64B5DDB7138D}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="9270" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1514,7 +1514,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E49" sqref="E49"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3368,7 +3368,7 @@
         <v>71</v>
       </c>
       <c r="E47" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F47" s="30"/>
       <c r="G47" s="34"/>

</xml_diff>

<commit_message>
3.1.3 Update Orders table when order is placed
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="109_{21EAC73E-584B-4B3F-8E40-DD04FB917DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{7CE1B172-6143-4AD6-9A8F-64B5DDB7138D}"/>
+  <xr:revisionPtr revIDLastSave="44" documentId="109_{21EAC73E-584B-4B3F-8E40-DD04FB917DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E37278D4-329E-4257-A05A-4DD938103E85}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="9270" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="223">
   <si>
     <t>Confirm</t>
   </si>
@@ -720,6 +720,9 @@
   </si>
   <si>
     <t>62 // with 10%</t>
+  </si>
+  <si>
+    <t>Maybe</t>
   </si>
 </sst>
 </file>
@@ -1513,8 +1516,8 @@
   <dimension ref="A1:AC1121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1531,7 +1534,7 @@
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; I172 &amp; "  /  Verified: " &amp; J172 &amp; "  /  Verified with Deductions: " &amp; K172 &amp; "  /  Verified with Deductions &amp; Milestones: " &amp; L172</f>
-        <v>Unverified Marks: 58  /  Verified: 58  /  Verified with Deductions: 52  /  Verified with Deductions &amp; Milestones: 70</v>
+        <v>Unverified Marks: 66  /  Verified: 58  /  Verified with Deductions: 52  /  Verified with Deductions &amp; Milestones: 70</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -3286,7 +3289,7 @@
       </c>
       <c r="E45" s="11"/>
       <c r="F45" s="25" t="s">
-        <v>20</v>
+        <v>222</v>
       </c>
       <c r="G45" s="26">
         <v>8</v>
@@ -3296,7 +3299,7 @@
       </c>
       <c r="I45" s="21">
         <f>IF(OR(F45 = "maybe", F45 = "yes"),G45, 0)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J45" s="21">
         <f>IF(F45 = "yes",G45, 0)</f>
@@ -3333,7 +3336,7 @@
         <v>70</v>
       </c>
       <c r="E46" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F46" s="30"/>
       <c r="G46" s="34"/>
@@ -3438,7 +3441,7 @@
         <v>73</v>
       </c>
       <c r="E49" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F49" s="30"/>
       <c r="G49" s="34"/>
@@ -3473,7 +3476,7 @@
         <v>74</v>
       </c>
       <c r="E50" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F50" s="30"/>
       <c r="G50" s="34"/>
@@ -8135,7 +8138,7 @@
       <c r="H172" s="11"/>
       <c r="I172" s="58">
         <f t="shared" ref="I172:K172" si="23">SUM(I4:I164)</f>
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="J172" s="28">
         <f t="shared" si="23"/>

</xml_diff>

<commit_message>
Final commit. Fix various bugs with storing and updating orders and users in active admin. Update checkout controller and views for consistancy.
</commit_message>
<xml_diff>
--- a/Full Stack - Ecommerce Project Marking Sheet.xlsx
+++ b/Full Stack - Ecommerce Project Marking Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iande\OneDrive\Documents\RRC\FallTerm2020\Adev-2007_FullStack\EcommerceProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="109_{21EAC73E-584B-4B3F-8E40-DD04FB917DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{E37278D4-329E-4257-A05A-4DD938103E85}"/>
+  <xr:revisionPtr revIDLastSave="60" documentId="109_{21EAC73E-584B-4B3F-8E40-DD04FB917DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A0D0EE01-93DD-4A78-8155-6C4DBAF33328}"/>
   <bookViews>
     <workbookView xWindow="-28800" yWindow="9270" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1516,8 +1516,8 @@
   <dimension ref="A1:AC1121"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1534,7 +1534,7 @@
     <row r="1" spans="1:29" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="str">
         <f>"Unverified Marks: " &amp; I172 &amp; "  /  Verified: " &amp; J172 &amp; "  /  Verified with Deductions: " &amp; K172 &amp; "  /  Verified with Deductions &amp; Milestones: " &amp; L172</f>
-        <v>Unverified Marks: 66  /  Verified: 58  /  Verified with Deductions: 52  /  Verified with Deductions &amp; Milestones: 70</v>
+        <v>Unverified Marks: 82  /  Verified: 58  /  Verified with Deductions: 52  /  Verified with Deductions &amp; Milestones: 70</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -4030,7 +4030,7 @@
     </row>
     <row r="65" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A65" s="8"/>
-      <c r="B65" s="8"/>
+      <c r="B65" s="61"/>
       <c r="C65" s="23" t="s">
         <v>92</v>
       </c>
@@ -4039,7 +4039,7 @@
       </c>
       <c r="E65" s="11"/>
       <c r="F65" s="25" t="s">
-        <v>20</v>
+        <v>222</v>
       </c>
       <c r="G65" s="26">
         <v>2</v>
@@ -4047,7 +4047,7 @@
       <c r="H65" s="32"/>
       <c r="I65" s="21">
         <f>IF(OR(F65 = "maybe", F65 = "yes"),G65, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J65" s="21">
         <f>IF(F65 = "yes",G65, 0)</f>
@@ -4084,7 +4084,7 @@
         <v>94</v>
       </c>
       <c r="E66" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F66" s="30"/>
       <c r="G66" s="34"/>
@@ -4119,7 +4119,7 @@
         <v>95</v>
       </c>
       <c r="E67" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F67" s="30"/>
       <c r="G67" s="34"/>
@@ -4154,7 +4154,7 @@
         <v>96</v>
       </c>
       <c r="E68" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F68" s="30"/>
       <c r="G68" s="34"/>
@@ -4189,7 +4189,7 @@
         <v>97</v>
       </c>
       <c r="E69" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F69" s="30"/>
       <c r="G69" s="34"/>
@@ -4227,7 +4227,7 @@
       </c>
       <c r="E70" s="11"/>
       <c r="F70" s="25" t="s">
-        <v>20</v>
+        <v>222</v>
       </c>
       <c r="G70" s="26">
         <v>2</v>
@@ -4235,7 +4235,7 @@
       <c r="H70" s="32"/>
       <c r="I70" s="21">
         <f>IF(OR(F70 = "maybe", F70 = "yes"),G70, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J70" s="21">
         <f>IF(F70 = "yes",G70, 0)</f>
@@ -4272,7 +4272,7 @@
         <v>100</v>
       </c>
       <c r="E71" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F71" s="30"/>
       <c r="G71" s="34"/>
@@ -4378,7 +4378,7 @@
       </c>
       <c r="E74" s="11"/>
       <c r="F74" s="25" t="s">
-        <v>20</v>
+        <v>222</v>
       </c>
       <c r="G74" s="26">
         <v>6</v>
@@ -4386,7 +4386,7 @@
       <c r="H74" s="32"/>
       <c r="I74" s="21">
         <f>IF(OR(F74 = "maybe", F74 = "yes"),G74, 0)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="J74" s="21">
         <f>IF(F74 = "yes",G74, 0)</f>
@@ -4493,7 +4493,7 @@
         <v>106</v>
       </c>
       <c r="E77" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F77" s="30"/>
       <c r="G77" s="34"/>
@@ -4566,7 +4566,7 @@
       </c>
       <c r="E79" s="11"/>
       <c r="F79" s="25" t="s">
-        <v>20</v>
+        <v>222</v>
       </c>
       <c r="G79" s="26">
         <v>2</v>
@@ -4574,7 +4574,7 @@
       <c r="H79" s="32"/>
       <c r="I79" s="21">
         <f>IF(OR(F79 = "maybe", F79 = "yes"),G79, 0)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J79" s="21">
         <f>IF(F79 = "yes",G79, 0)</f>
@@ -4611,7 +4611,7 @@
         <v>110</v>
       </c>
       <c r="E80" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F80" s="30"/>
       <c r="G80" s="34"/>
@@ -5760,7 +5760,7 @@
     </row>
     <row r="110" spans="1:29" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A110" s="8"/>
-      <c r="B110" s="61"/>
+      <c r="B110" s="62"/>
       <c r="C110" s="23" t="s">
         <v>144</v>
       </c>
@@ -6264,7 +6264,7 @@
       </c>
       <c r="E122" s="11"/>
       <c r="F122" s="25" t="s">
-        <v>20</v>
+        <v>222</v>
       </c>
       <c r="G122" s="26">
         <v>4</v>
@@ -6274,7 +6274,7 @@
       </c>
       <c r="I122" s="21">
         <f>IF(OR(F122 = "maybe", F122 = "yes"),G122, 0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J122" s="21">
         <f>IF(F122 = "yes",G122, 0)</f>
@@ -6346,7 +6346,7 @@
         <v>163</v>
       </c>
       <c r="E124" s="25" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="F124" s="30"/>
       <c r="G124" s="34"/>
@@ -8138,7 +8138,7 @@
       <c r="H172" s="11"/>
       <c r="I172" s="58">
         <f t="shared" ref="I172:K172" si="23">SUM(I4:I164)</f>
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="J172" s="28">
         <f t="shared" si="23"/>

</xml_diff>